<commit_message>
Add ability for multiple years on one chart
Updated main code and reference xls/csv to have multiple years on one chart to show progression.
Only years with values are shown
So, students starting in a later year will work
Designed for Year 3,4,5 and 6.
With different colour line for each year with the latest year to the front.
</commit_message>
<xml_diff>
--- a/spider_data_points.xlsx
+++ b/spider_data_points.xlsx
@@ -5,55 +5,60 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="spider_data_points" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="spider_data_points_previous" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Code Captain X</t>
-  </si>
-  <si>
-    <t>Code Captain Y</t>
-  </si>
-  <si>
-    <t>Net Ninja X</t>
-  </si>
-  <si>
-    <t>Net Ninja Y</t>
-  </si>
-  <si>
-    <t>Searching Superstar X</t>
-  </si>
-  <si>
-    <t>Searching Superstar Y</t>
-  </si>
-  <si>
-    <t>Logic Leader X</t>
-  </si>
-  <si>
-    <t>Logic Leader Y</t>
-  </si>
-  <si>
-    <t>Tech Team X</t>
-  </si>
-  <si>
-    <t>Tech Team Y</t>
-  </si>
-  <si>
-    <t>Hardware Hero X</t>
-  </si>
-  <si>
-    <t>Hardware Hero Y</t>
+    <t xml:space="preserve">Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code Captain X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code Captain Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Ninja X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Ninja Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searching Superstar X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searching Superstar Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logic Leader X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logic Leader Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algo Ace X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algo Ace Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardware Hero X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardware Hero Y</t>
   </si>
 </sst>
 </file>
@@ -61,12 +66,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
-      <name val="DejaVu Sans"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -149,27 +154,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.91517857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7008928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5758928571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3080357142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1830357142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.2276785714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1026785714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8214285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6919642857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9375"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8125"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.5848214285714"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.4598214285714"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -215,298 +221,257 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1390</v>
+        <v>1690</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>910</v>
+        <v>969</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1810</v>
+        <v>1860</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>901</v>
+        <v>968</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2020</v>
+        <v>1925</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1810</v>
+        <v>1860</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>1645</v>
+        <v>1275</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>1390</v>
+        <v>1690</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>1645</v>
+        <v>1275</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>1180</v>
+        <v>1625</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1333</v>
+        <v>1627</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>807</v>
+        <v>852</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1867</v>
+        <v>1920</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>807</v>
+        <v>852</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>2140</v>
+        <v>2040</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>1870</v>
+        <v>1920</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>1745</v>
+        <v>1390</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>1330</v>
+        <v>1627</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>1745</v>
+        <v>1390</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>1060</v>
+        <v>1508</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1265</v>
+        <v>1563</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>684</v>
+        <v>734</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1938</v>
+        <v>1986</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>684</v>
+        <v>735</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>2280</v>
+        <v>2158</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>1940</v>
+        <v>1986</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>1870</v>
+        <v>1507</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>1265</v>
+        <v>1563</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>1870</v>
+        <v>1507</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>920</v>
+        <v>1392</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1189</v>
+        <v>1500</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>549</v>
+        <v>617</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2019</v>
+        <v>2048</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>549</v>
+        <v>620</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>2440</v>
+        <v>2275</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>2015</v>
+        <v>2048</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>2005</v>
+        <v>1622</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>1185</v>
+        <v>1500</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>2005</v>
+        <v>1622</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>766</v>
+        <v>1275</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1111</v>
+        <v>1438</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>416</v>
+        <v>502</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>2089</v>
+        <v>2110</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>416</v>
+        <v>503</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>2590</v>
+        <v>2390</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>2095</v>
+        <v>2110</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>2135</v>
+        <v>1740</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>1115</v>
+        <v>1438</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>2135</v>
+        <v>1740</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>614</v>
+        <v>1157</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1044</v>
+        <v>1375</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>289</v>
+        <v>386</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>2161</v>
+        <v>2170</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>289</v>
+        <v>386</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>2730</v>
+        <v>2515</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>2160</v>
+        <v>2170</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>2265</v>
+        <v>1858</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>1045</v>
+        <v>1375</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>2265</v>
+        <v>1858</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>465</v>
+        <v>1033</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>1044</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>289</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>2161</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>289</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>2730</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>1276</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>2160</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>2265</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>1045</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>2265</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>465</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <v>1276</v>
+        <v>1120</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>